<commit_message>
New Summary Stats File
</commit_message>
<xml_diff>
--- a/Ryan/Repository/GCData_LP_FAME w Conc Data - Apr 2021.xlsx
+++ b/Ryan/Repository/GCData_LP_FAME w Conc Data - Apr 2021.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Baopa\Documents\Pfleger_Lab\BTE_Mutagenesis\GC_Data\Apr_2021\Landing_Pad\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Baopa\Documents\GitHub\GC_Code\Ryan\Repository\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{423650E5-499B-420D-BBE1-CCEB8D7C0319}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64E8E588-7BA9-4D2F-ADAC-0345EE9DF151}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15000" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="John_Code" sheetId="1" r:id="rId1"/>
@@ -2229,7 +2229,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F480"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A186" workbookViewId="0">
+      <selection activeCell="F194" sqref="F194:F204"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -11337,7 +11339,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F267"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A219" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -22163,7 +22165,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F285"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="A115" sqref="A115"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -27877,7 +27881,7 @@
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -28381,11 +28385,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:J286"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A164" workbookViewId="0">
-      <selection activeCell="E192" sqref="E192"/>
+    <sheetView tabSelected="1" topLeftCell="A114" workbookViewId="0">
+      <selection activeCell="N118" sqref="N118:N128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="6" max="6" width="32.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="2">

</xml_diff>